<commit_message>
updated with new data changes
</commit_message>
<xml_diff>
--- a/Harvard’s Endowment/data/multi_asset_etf_data.xlsx
+++ b/Harvard’s Endowment/data/multi_asset_etf_data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shinjikuno/GitRepositories/FINM 36700 Portfolio and Risk Management/Harvard’s Endowment/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhendricks/Projects/finm-portfolio/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6172D-E9AF-E347-B14E-C291F96FD9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458A557E-CD97-7F44-B148-6191FC73FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31260" yWindow="-16480" windowWidth="30240" windowHeight="17840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="descriptions" sheetId="1" r:id="rId1"/>
+    <sheet name="descriptions" sheetId="5" r:id="rId1"/>
     <sheet name="prices" sheetId="2" r:id="rId2"/>
     <sheet name="total returns" sheetId="3" r:id="rId3"/>
     <sheet name="excess returns" sheetId="4" r:id="rId4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>ticker</t>
   </si>
@@ -131,6 +131,36 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>The trust seeks to achieve its investment objective by holding a portfolio of the common stocks that are included in the index, with the weight of each stock in the portfolio substantially corresponding to the weight of such stock in the index.</t>
+  </si>
+  <si>
+    <t>The fund generally will invest at least 80% of its assets in the component securities of its underlying index and in investments that have economic characteristics that are substantially identical to the component securities of its underlying index. The index is a free float-adjusted, market capitalization-weighted index designed to measure large- and mid-capitalization equity market performance of developed markets outside of the U.S. and Canada.</t>
+  </si>
+  <si>
+    <t>The fund generally will invest at least 80% of its assets in the component securities of its underlying index and in investments that have economic characteristics that are substantially identical to the component securities of its underlying index. The index is designed to measure equity market performance in the global emerging markets. The underlying index includes large- and mid-capitalization companies and may change over time.</t>
+  </si>
+  <si>
+    <t>The fund generally will invest at least 90% of its total assets in securities (including American depositary receipts ("ADRs") and global depositary receipts ("GDRs")) that comprise the underlying index. The underlying index is composed of securities, ADRs and GDRs of 40 to 75 private equity companies, including business development companies ("BDCs"), master limited partnerships ("MLPs"), alternative asset managers and other entities that are listed on a nationally recognized exchange.</t>
+  </si>
+  <si>
+    <t>The fund is a "fund of funds" which means it invests, under normal circumstances, at least 80% of its net assets, plus the amount of any borrowings for investment purposes, in the investments included in its underlying index, which includes underlying funds. The underlying index consists of a number of components ("underlying index Components") selected in accordance with its rules-based methodology of such underlying index.</t>
+  </si>
+  <si>
+    <t>The underlying index is a rules-based index consisting of U.S. dollar-denominated, high yield corporate bonds for sale in the U.S. The fund will invest at least 80% of its assets in the component securities of the underlying index, and the fund will invest at least 90% of its assets in fixed income securities of the types included in the underlying index that the advisor believes will help the fund track the underlying index.</t>
+  </si>
+  <si>
+    <t>The fund pursues its investment objective by investing in a portfolio of exchange-traded futures on Light Sweet Crude Oil (WTI), Heating Oil, RBOB Gasoline, Natural Gas, Brent Crude, Gold, Silver, Aluminum, Zinc, Copper Grade A, Corn, Wheat, Soybeans, and Sugar. The index is composed of notional amounts of each of these commodities.</t>
+  </si>
+  <si>
+    <t>The fund generally invests substantially all, but at least 80%, of its total assets in the securities comprising the index and in securities that the Adviser determines have economic characteristics that are substantially identical to the economic characteristics of the securities that comprise the index. The index is designed to track the fixed-rate local currency sovereign debt of investment grade countries outside the United States. It is non-diversified.</t>
+  </si>
+  <si>
+    <t>The index tracks the performance of inflation-protected public obligations of the U.S. Treasury, commonly known as “TIPS,” that have a remaining maturity of more than one year. The fund will invest at least 80% of its assets in the component securities of the index, and it will invest at least 90% of its assets in U.S. Treasury securities that BFA believes will help the fund track the index.</t>
+  </si>
+  <si>
+    <t>The fund will invest at least 80% of its assets in the component securities of the underlying index, and it will invest at least 90% of its assets in U.S. Treasury securities that BFA believes will help the fund track the underlying index. The index measures the performance of public obligations of the U.S. Treasury that have a remaining maturity of less than or equal to one year.</t>
   </si>
 </sst>
 </file>
@@ -499,10 +529,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0548E9F-AA47-3B46-B903-B92960E1DD5C}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -542,6 +572,15 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="E2">
+        <v>24710239</v>
+      </c>
+      <c r="F2">
+        <v>603516960768</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -556,6 +595,15 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3">
+        <v>4818965</v>
+      </c>
+      <c r="F3">
+        <v>63209721856</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -570,6 +618,15 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4">
+        <v>8563600</v>
+      </c>
+      <c r="F4">
+        <v>17162833920</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -584,6 +641,15 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
+      <c r="E5">
+        <v>3622</v>
+      </c>
+      <c r="F5">
+        <v>258060880</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -598,6 +664,15 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
+      <c r="E6">
+        <v>12559</v>
+      </c>
+      <c r="F6">
+        <v>696944896</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -612,6 +687,15 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
+      <c r="E7">
+        <v>19724563</v>
+      </c>
+      <c r="F7">
+        <v>15944028160</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -626,6 +710,15 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
+      <c r="E8">
+        <v>184605</v>
+      </c>
+      <c r="F8">
+        <v>1142769792</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -641,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>6211444</v>
+        <v>2170005</v>
       </c>
       <c r="F9">
         <v>3480166144</v>
@@ -664,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="E10">
-        <v>7506784</v>
+        <v>5269754</v>
       </c>
       <c r="F10">
         <v>34938195968</v>
@@ -686,6 +779,15 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
+      <c r="E11">
+        <v>155330</v>
+      </c>
+      <c r="F11">
+        <v>1423427840</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -700,6 +802,15 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
+      <c r="E12">
+        <v>1601034</v>
+      </c>
+      <c r="F12">
+        <v>13900867584</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -713,6 +824,15 @@
       </c>
       <c r="D13" t="s">
         <v>10</v>
+      </c>
+      <c r="E13">
+        <v>2043964</v>
+      </c>
+      <c r="F13">
+        <v>20599980032</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -727,9 +847,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -7877,9 +7994,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -14983,12 +15097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>